<commit_message>
Zeitprotokolle hinzugefügt. Besprechungsprotokolle zusammengefügt.
</commit_message>
<xml_diff>
--- a/protokolle/zeitaufzeichnung/srnka.xlsx
+++ b/protokolle/zeitaufzeichnung/srnka.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juergen\repositories\SimpleQ\protokolle\zeitaufzeichnung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE593B84-C356-4E1E-B096-10A95604DE66}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E930253-2A62-4743-BAE9-543179C3D66C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5820" yWindow="1065" windowWidth="25365" windowHeight="14850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diplomprojekt" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="65">
   <si>
     <t>Zeitaufzeichnung SimpleQ</t>
   </si>
@@ -64,9 +64,6 @@
     <t>Gesamt (h)</t>
   </si>
   <si>
-    <t>www.tmetric.com, 29.03.2019</t>
-  </si>
-  <si>
     <t>bpmn</t>
   </si>
   <si>
@@ -151,9 +148,6 @@
     <t>Nico Srnka</t>
   </si>
   <si>
-    <t>vertriebshomepage</t>
-  </si>
-  <si>
     <t>Implementierung</t>
   </si>
   <si>
@@ -161,6 +155,75 @@
   </si>
   <si>
     <t>Diplomschrift nachtrag urlaub</t>
+  </si>
+  <si>
+    <t>website grundgerüst idee</t>
+  </si>
+  <si>
+    <t>website grundgerüst</t>
+  </si>
+  <si>
+    <t>website smooth scroll, handy</t>
+  </si>
+  <si>
+    <t>website form</t>
+  </si>
+  <si>
+    <t>website section paddings</t>
+  </si>
+  <si>
+    <t>website section anordnung</t>
+  </si>
+  <si>
+    <t>webinterface settings, support grundidee</t>
+  </si>
+  <si>
+    <t>webinterface projekt bugfix</t>
+  </si>
+  <si>
+    <t>webinterface setting grundgerüst</t>
+  </si>
+  <si>
+    <t>webinterface support grundgerüst</t>
+  </si>
+  <si>
+    <t>website fixes, handy steuern bug</t>
+  </si>
+  <si>
+    <t>webinterface settings benutzerinformationen fix</t>
+  </si>
+  <si>
+    <t>webinterface support form, support faq, settings abrechnungsdatum</t>
+  </si>
+  <si>
+    <t>webinterface settings benutzerinformationen fix, fehlerbehebung ajax calls</t>
+  </si>
+  <si>
+    <t>webinterface fehlermeldungen / hilfestellungen</t>
+  </si>
+  <si>
+    <t>webinterface aktivierte modi fixes und modals</t>
+  </si>
+  <si>
+    <t>webinterface settings design änderung</t>
+  </si>
+  <si>
+    <t>webinterface ajax call fehlerbehebung</t>
+  </si>
+  <si>
+    <t>webinterface support fields kontaktformular, settings navigation</t>
+  </si>
+  <si>
+    <t>website handy fixes, responsive fixes</t>
+  </si>
+  <si>
+    <t>website form fix</t>
+  </si>
+  <si>
+    <t>www.tmetric.com, 30.03.2019</t>
+  </si>
+  <si>
+    <t>vertriebshomepage backgrounds, start page header</t>
   </si>
 </sst>
 </file>
@@ -168,7 +231,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -696,7 +759,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -747,24 +810,20 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="46" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1121,33 +1180,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C78"/>
+  <dimension ref="A1:C83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="66" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="19" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
+      <c r="B1" s="22"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="20"/>
+        <v>38</v>
+      </c>
+      <c r="C2" s="19"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -1156,31 +1215,31 @@
       <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="20"/>
+      <c r="C3" s="19"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="20"/>
+        <v>63</v>
+      </c>
+      <c r="C4" s="19"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="7">
-        <f>C78</f>
-        <v>7.9930555555555562</v>
-      </c>
-      <c r="C5" s="20"/>
+        <f>C83</f>
+        <v>8.0798611111111125</v>
+      </c>
+      <c r="C5" s="19"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="8"/>
-      <c r="C6" s="20"/>
+      <c r="C6" s="19"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -1189,7 +1248,7 @@
       <c r="B7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="20" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1198,7 +1257,7 @@
         <v>43300</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="15">
         <v>4.1666666666666664E-2</v>
@@ -1209,7 +1268,7 @@
         <v>43309</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="15">
         <v>8.3333333333333329E-2</v>
@@ -1220,7 +1279,7 @@
         <v>43327</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="15">
         <v>4.1666666666666664E-2</v>
@@ -1231,7 +1290,7 @@
         <v>43334</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="C11" s="15">
         <v>0.20833333333333334</v>
@@ -1242,7 +1301,7 @@
         <v>43347</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="C12" s="15">
         <v>0.20833333333333334</v>
@@ -1253,293 +1312,293 @@
         <v>43354</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="C13" s="15">
-        <v>0.12569444444444444</v>
+        <v>8.4027777777777771E-2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="14">
-        <v>43358</v>
+        <v>43354</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="15">
-        <v>8.3333333333333329E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="14">
-        <v>43361</v>
+        <v>43358</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="C15" s="15">
-        <v>0.13958333333333334</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
-        <v>43365</v>
+        <v>43361</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" s="15">
-        <v>2.4999999999999998E-2</v>
+        <v>0.13958333333333334</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="14">
-        <v>43368</v>
+        <v>43365</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C17" s="15">
-        <v>0.12986111111111112</v>
+        <v>2.4999999999999998E-2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="14">
-        <v>43372</v>
+        <v>43368</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="C18" s="15">
-        <v>5.0694444444444452E-2</v>
+        <v>6.5277777777777782E-2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="14">
-        <v>43379</v>
+        <v>43368</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C19" s="15">
-        <v>0.125</v>
+        <v>6.458333333333334E-2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="14">
-        <v>43380</v>
+        <v>43372</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C20" s="15">
-        <v>3.0555555555555555E-2</v>
+        <v>5.0694444444444452E-2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="14">
-        <v>43382</v>
+        <v>43379</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="C21" s="15">
-        <v>0.15555555555555556</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="14">
-        <v>43385</v>
+        <v>43380</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="C22" s="15">
-        <v>0.15625</v>
+        <v>3.0555555555555555E-2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="14">
-        <v>43389</v>
+        <v>43382</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="C23" s="15">
-        <v>0.18611111111111112</v>
+        <v>7.9861111111111105E-2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="14">
-        <v>43396</v>
+        <v>43382</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="C24" s="15">
-        <v>0.23958333333333334</v>
+        <v>7.5694444444444439E-2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="14">
-        <v>43399</v>
+        <v>43385</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C25" s="15">
-        <v>0.10347222222222223</v>
+        <v>0.15625</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="14">
-        <v>43401</v>
+        <v>43389</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C26" s="15">
-        <v>0.12638888888888888</v>
+        <v>0.18611111111111112</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="14">
-        <v>43408</v>
+        <v>43396</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="C27" s="15">
-        <v>8.6805555555555566E-2</v>
+        <v>0.23958333333333334</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="14">
-        <v>43408</v>
+        <v>43399</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C28" s="15">
-        <v>8.1250000000000003E-2</v>
+        <v>0.10347222222222223</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="14">
-        <v>43409</v>
+        <v>43401</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C29" s="15">
-        <v>7.1527777777777787E-2</v>
+        <v>0.12638888888888888</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="14">
-        <v>43410</v>
+        <v>43408</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C30" s="15">
-        <v>0.43958333333333338</v>
+        <v>8.6805555555555566E-2</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="14">
-        <v>43417</v>
+        <v>43408</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="C31" s="15">
-        <v>0.27777777777777779</v>
+        <v>8.1250000000000003E-2</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="14">
-        <v>43419</v>
+        <v>43409</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C32" s="15">
-        <v>8.6805555555555566E-2</v>
+        <v>7.1527777777777787E-2</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="14">
-        <v>43424</v>
+        <v>43410</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C33" s="15">
-        <v>0.20833333333333334</v>
+        <v>0.43958333333333338</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="14">
-        <v>43425</v>
+        <v>43417</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="C34" s="15">
-        <v>0.14583333333333334</v>
+        <v>0.27777777777777779</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="14">
-        <v>43429</v>
+        <v>43419</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="C35" s="15">
-        <v>5.2777777777777778E-2</v>
+        <v>8.6805555555555566E-2</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="14">
-        <v>43438</v>
+        <v>43424</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C36" s="15">
-        <v>0.16666666666666666</v>
+        <v>0.20833333333333334</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="14">
-        <v>43443</v>
+        <v>43425</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="C37" s="15">
-        <v>0.16666666666666666</v>
+        <v>0.14583333333333334</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="14">
-        <v>43444</v>
+        <v>43429</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C38" s="15">
-        <v>4.1666666666666664E-2</v>
+        <v>5.2777777777777778E-2</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="14">
-        <v>43445</v>
+        <v>43438</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="C39" s="15">
         <v>0.16666666666666666</v>
@@ -1547,32 +1606,32 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="14">
-        <v>43454</v>
+        <v>43443</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="C40" s="15">
-        <v>0.12847222222222224</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="14">
-        <v>43464</v>
+        <v>43444</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="C41" s="15">
-        <v>0.16180555555555556</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="14">
-        <v>43473</v>
+        <v>43445</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="C42" s="15">
         <v>0.16666666666666666</v>
@@ -1580,175 +1639,175 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="14">
-        <v>43475</v>
+        <v>43454</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="C43" s="15">
-        <v>8.6805555555555566E-2</v>
+        <v>0.12847222222222224</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="14">
-        <v>43475</v>
+        <v>43464</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C44" s="15">
-        <v>8.3333333333333329E-2</v>
+        <v>0.16180555555555556</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="14">
-        <v>43476</v>
+        <v>43473</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C45" s="15">
-        <v>6.7361111111111108E-2</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="14">
-        <v>43477</v>
+        <v>43475</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C46" s="15">
-        <v>0.10625</v>
+        <v>8.6805555555555566E-2</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="14">
-        <v>43478</v>
+        <v>43475</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C47" s="15">
-        <v>0.1173611111111111</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="14">
-        <v>43479</v>
+        <v>43476</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C48" s="15">
-        <v>6.6666666666666666E-2</v>
+        <v>6.7361111111111108E-2</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="14">
-        <v>43480</v>
+        <v>43477</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C49" s="15">
-        <v>0.15416666666666667</v>
+        <v>0.10625</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="14">
-        <v>43482</v>
+        <v>43478</v>
       </c>
       <c r="B50" s="17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C50" s="15">
-        <v>7.6388888888888895E-2</v>
+        <v>0.1173611111111111</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="14">
-        <v>43487</v>
+        <v>43479</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C51" s="15">
-        <v>8.3333333333333329E-2</v>
+        <v>6.6666666666666666E-2</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="14">
-        <v>43489</v>
+        <v>43480</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C52" s="15">
-        <v>7.5694444444444439E-2</v>
+        <v>0.15416666666666667</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="14">
-        <v>43490</v>
+        <v>43482</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C53" s="15">
-        <v>0.10416666666666667</v>
+        <v>7.6388888888888895E-2</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="14">
-        <v>43490</v>
+        <v>43487</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C54" s="15">
-        <v>4.6527777777777779E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="14">
-        <v>43491</v>
+        <v>43489</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C55" s="15">
-        <v>0.17013888888888887</v>
+        <v>7.5694444444444439E-2</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="14">
-        <v>43493</v>
+        <v>43490</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C56" s="15">
-        <v>7.0833333333333331E-2</v>
+        <v>0.10416666666666667</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="14">
-        <v>43494</v>
+        <v>43490</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C57" s="15">
-        <v>0.11805555555555557</v>
+        <v>4.6527777777777779E-2</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="14">
-        <v>43496</v>
+        <v>43491</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C58" s="15">
         <v>0.17013888888888887</v>
@@ -1756,43 +1815,43 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="14">
-        <v>43507</v>
+        <v>43493</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C59" s="15">
-        <v>4.9999999999999996E-2</v>
+        <v>7.0833333333333331E-2</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="14">
-        <v>43508</v>
+        <v>43494</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C60" s="15">
-        <v>3.6111111111111115E-2</v>
+        <v>0.11805555555555557</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="14">
-        <v>43511</v>
+        <v>43496</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C61" s="15">
-        <v>0.14305555555555557</v>
+        <v>0.17013888888888887</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="14">
-        <v>43515</v>
+        <v>43507</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C62" s="15">
         <v>4.9999999999999996E-2</v>
@@ -1800,177 +1859,232 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="14">
-        <v>43518</v>
+        <v>43508</v>
       </c>
       <c r="B63" s="17" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C63" s="15">
-        <v>4.3055555555555562E-2</v>
+        <v>3.6111111111111115E-2</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="14">
-        <v>43522</v>
+        <v>43511</v>
       </c>
       <c r="B64" s="17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C64" s="15">
-        <v>8.6805555555555566E-2</v>
+        <v>0.14305555555555557</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="14">
-        <v>43526</v>
+        <v>43515</v>
       </c>
       <c r="B65" s="17" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C65" s="15">
-        <v>0.19930555555555554</v>
+        <v>4.9999999999999996E-2</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="14">
-        <v>43529</v>
+        <v>43518</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C66" s="15">
-        <v>0.1111111111111111</v>
+        <v>4.3055555555555562E-2</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="14">
-        <v>43530</v>
+        <v>43522</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C67" s="15">
-        <v>5.7638888888888885E-2</v>
+        <v>8.6805555555555566E-2</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="14">
-        <v>43531</v>
+        <v>43526</v>
       </c>
       <c r="B68" s="17" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C68" s="15">
-        <v>0.11319444444444444</v>
+        <v>0.19930555555555554</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="14">
-        <v>43533</v>
+        <v>43529</v>
       </c>
       <c r="B69" s="17" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C69" s="15">
-        <v>0.13749999999999998</v>
+        <v>0.1111111111111111</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="14">
-        <v>43534</v>
+        <v>43530</v>
       </c>
       <c r="B70" s="17" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C70" s="15">
-        <v>0.14583333333333334</v>
+        <v>5.7638888888888885E-2</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="14">
-        <v>43535</v>
+        <v>43531</v>
       </c>
       <c r="B71" s="17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C71" s="15">
-        <v>4.4444444444444446E-2</v>
+        <v>0.11319444444444444</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="14">
-        <v>43536</v>
+        <v>43533</v>
       </c>
       <c r="B72" s="17" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C72" s="15">
-        <v>0.1111111111111111</v>
+        <v>0.13749999999999998</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="14">
-        <v>43537</v>
+        <v>43534</v>
       </c>
       <c r="B73" s="17" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C73" s="15">
-        <v>8.6805555555555566E-2</v>
+        <v>0.14583333333333334</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="14">
-        <v>43538</v>
+        <v>43535</v>
       </c>
       <c r="B74" s="17" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C74" s="15">
-        <v>4.5138888888888888E-2</v>
+        <v>4.4444444444444446E-2</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="14">
-        <v>43540</v>
+        <v>43536</v>
       </c>
       <c r="B75" s="17" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C75" s="15">
-        <v>0.1451388888888889</v>
+        <v>0.1111111111111111</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="14">
-        <v>43543</v>
+        <v>43537</v>
       </c>
       <c r="B76" s="17" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C76" s="15">
-        <v>3.4722222222222224E-2</v>
+        <v>8.6805555555555566E-2</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="14">
-        <v>43551</v>
+        <v>43538</v>
       </c>
       <c r="B77" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C77" s="15">
         <v>4.5138888888888888E-2</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="23"/>
-      <c r="B78" s="22" t="s">
+      <c r="A78" s="14">
+        <v>43540</v>
+      </c>
+      <c r="B78" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C78" s="15">
+        <v>0.1451388888888889</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="14">
+        <v>43543</v>
+      </c>
+      <c r="B79" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C79" s="15">
+        <v>3.4722222222222224E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="14">
+        <v>43551</v>
+      </c>
+      <c r="B80" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C80" s="15">
+        <v>4.5138888888888888E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="14">
+        <v>43553</v>
+      </c>
+      <c r="B81" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C81" s="15">
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="14">
+        <v>43554</v>
+      </c>
+      <c r="B82" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C82" s="15">
+        <v>4.5138888888888888E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="16"/>
+      <c r="B83" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C78" s="24">
-        <f>SUM(C8:C77)</f>
-        <v>7.9930555555555562</v>
+      <c r="C83" s="21">
+        <f>SUM(C8:C82)</f>
+        <v>8.0798611111111125</v>
       </c>
     </row>
   </sheetData>
@@ -1986,8 +2100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1998,17 +2112,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
+      <c r="B1" s="22"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="6"/>
     </row>
@@ -2026,7 +2140,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="C4" s="6"/>
     </row>
@@ -2061,7 +2175,7 @@
         <v>43399</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="C8" s="15">
         <v>0.12916666666666668</v>
@@ -2105,7 +2219,7 @@
         <v>43465</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C12" s="15">
         <v>7.2916666666666671E-2</v>
@@ -2116,7 +2230,7 @@
         <v>43466</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C13" s="15">
         <v>2.6388888888888889E-2</v>
@@ -2127,7 +2241,7 @@
         <v>43470</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C14" s="15">
         <v>3.6111111111111115E-2</v>
@@ -2149,7 +2263,7 @@
         <v>43508</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C16" s="15">
         <v>0.20833333333333334</v>

</xml_diff>